<commit_message>
broker population added and set.
</commit_message>
<xml_diff>
--- a/RalloCloud/data/PoPs.xlsx
+++ b/RalloCloud/data/PoPs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="83">
   <si>
     <t>DFN</t>
   </si>
@@ -257,6 +257,12 @@
   </si>
   <si>
     <t>NORDUNET</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Denmark</t>
   </si>
 </sst>
 </file>
@@ -623,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,16 +640,17 @@
     <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>78</v>
       </c>
@@ -656,32 +663,35 @@
       <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -694,32 +704,35 @@
       <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="4">
+      <c r="H2" s="4">
         <v>2</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J2" s="5">
-        <v>1538</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="5">
+        <v>1538</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -732,32 +745,35 @@
       <c r="D3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3">
+        <v>81</v>
+      </c>
+      <c r="F3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3" s="4">
         <v>2</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>69</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J3" s="5">
-        <v>1538</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="5">
+        <v>1538</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -770,32 +786,35 @@
       <c r="D4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="4">
         <v>2</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>69</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J4" s="5">
-        <v>1538</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="5">
+        <v>1538</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -808,32 +827,35 @@
       <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5">
         <v>30</v>
       </c>
       <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="4">
+      <c r="H5" s="4">
         <v>3</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>69</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J5" s="5">
-        <v>1538</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J5" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" s="5">
+        <v>1538</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -846,32 +868,35 @@
       <c r="D6" t="s">
         <v>32</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
         <v>34</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="4">
+      <c r="H6" s="4">
         <v>1</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>69</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J6" s="5">
-        <v>1538</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J6" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" s="5">
+        <v>1538</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -884,32 +909,35 @@
       <c r="D7" t="s">
         <v>36</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
         <v>39</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="4">
+      <c r="H7" s="4">
         <v>1</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>69</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J7" s="5">
-        <v>1538</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K7" s="5">
+        <v>1538</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -922,32 +950,35 @@
       <c r="D8" t="s">
         <v>44</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
         <v>45</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="4">
+      <c r="H8" s="4">
         <v>2</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J8" s="5">
-        <v>1538</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J8" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8" s="5">
+        <v>1538</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -960,32 +991,35 @@
       <c r="D9" t="s">
         <v>42</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
         <v>47</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="4">
+      <c r="H9" s="4">
         <v>2</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>69</v>
       </c>
-      <c r="I9" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J9" s="5">
-        <v>1538</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J9" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K9" s="5">
+        <v>1538</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -993,37 +1027,40 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
         <v>36</v>
       </c>
-      <c r="D10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
         <v>49</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="4">
+      <c r="H10" s="4">
         <v>1</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>69</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J10" s="5">
-        <v>1538</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J10" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K10" s="5">
+        <v>1538</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1036,32 +1073,35 @@
       <c r="D11" t="s">
         <v>52</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
         <v>53</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="4">
+      <c r="H11" s="4">
         <v>2</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>69</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J11" s="5">
-        <v>1538</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J11" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K11" s="5">
+        <v>1538</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1074,32 +1114,35 @@
       <c r="D12" t="s">
         <v>57</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
         <v>58</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="4">
+      <c r="H12" s="4">
         <v>1</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>69</v>
       </c>
-      <c r="I12" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J12" s="5">
-        <v>1538</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="L12" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J12" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K12" s="5">
+        <v>1538</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1112,32 +1155,35 @@
       <c r="D13" t="s">
         <v>28</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
         <v>30</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="4">
+      <c r="H13" s="4">
         <v>3</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>69</v>
       </c>
-      <c r="I13" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J13" s="5">
-        <v>1538</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J13" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K13" s="5">
+        <v>1538</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1150,32 +1196,35 @@
       <c r="D14" t="s">
         <v>60</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14">
+        <v>23</v>
+      </c>
+      <c r="F14" t="s">
         <v>61</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>62</v>
       </c>
-      <c r="G14" s="4">
+      <c r="H14" s="4">
         <v>1</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>69</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J14" s="5">
-        <v>1538</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J14" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K14" s="5">
+        <v>1538</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1188,37 +1237,46 @@
       <c r="D15" t="s">
         <v>63</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
         <v>65</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>66</v>
       </c>
-      <c r="G15" s="4">
+      <c r="H15" s="4">
         <v>1</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>69</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J15" s="5">
-        <v>1538</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J15" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K15" s="5">
+        <v>1538</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>80</v>
+      </c>
+      <c r="C16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>